<commit_message>
Correções do capítulo empírico: seção dos fatos estilizados
</commit_message>
<xml_diff>
--- a/Dados/Fatos_Estilizados/SCF_merged.xlsx
+++ b/Dados/Fatos_Estilizados/SCF_merged.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="gpetrini"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="5" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Housing_NW" sheetId="1" r:id="rId4"/>
@@ -19,17 +19,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1573936295" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1573936295" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1573936295" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1573936295"/>
+      <pm:revision xmlns:pm="smNativeData" day="1579466201" val="973" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1579466201" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1579466201" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1579466201"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
   <si>
     <t>Percentile of net worth</t>
   </si>
@@ -67,7 +67,7 @@
     <t>80–89.9</t>
   </si>
   <si>
-    <t>Percentil da renda</t>
+    <t>Percentil da Renda</t>
   </si>
   <si>
     <t>Imóveis</t>
@@ -76,10 +76,13 @@
     <t>Ações</t>
   </si>
   <si>
+    <t>Secundário</t>
+  </si>
+  <si>
     <t>Percentil da riqueza</t>
   </si>
   <si>
-    <t>Secundário</t>
+    <t>Percentil da renda</t>
   </si>
   <si>
     <t>Total</t>
@@ -110,7 +113,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -125,7 +128,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -141,7 +144,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Times New Roman" sz="220" lang="default" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" i="1"/>
@@ -156,7 +159,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Times New Roman" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -172,7 +175,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -188,7 +191,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -205,7 +208,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573936295" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1579466201" ulstyle="none" kern="1">
             <pm:latin face="Times New Roman" sz="220" lang="default" weight="bold" i="1"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" i="1"/>
@@ -214,7 +217,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,17 +246,6 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1573936295" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
@@ -269,10 +261,24 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1579466201" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -288,7 +294,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295"/>
+          <pm:border xmlns:pm="smNativeData" id="1579466201"/>
         </ext>
       </extLst>
     </border>
@@ -307,7 +313,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -328,7 +334,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -352,7 +358,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -375,7 +381,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -398,7 +404,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -421,7 +427,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -442,7 +448,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -455,36 +461,17 @@
       <right style="none">
         <color rgb="FF000000"/>
       </right>
-      <top style="none">
+      <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="none">
+      <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
-            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+            <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
       </extLst>
@@ -504,7 +491,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -525,7 +512,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -547,7 +534,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -569,7 +556,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -583,17 +570,59 @@
       <right style="none">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
+      <top style="none">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
+      <bottom style="none">
         <color rgb="FF000000"/>
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573936295">
+          <pm:border xmlns:pm="smNativeData" id="1579466201"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
+            <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+          </pm:border>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1579466201">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
+            <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
       </extLst>
@@ -602,14 +631,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -623,7 +652,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -634,7 +663,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -649,7 +678,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -666,7 +695,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -674,7 +703,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -682,7 +711,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -690,19 +719,43 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
+        </ext>
+      </extLst>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="2"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -710,31 +763,7 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -742,15 +771,16 @@
       <alignment horizontal="right" indent="2"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:cellMargin xmlns:pm="smNativeData" id="1573936295" l="0" r="384" t="0" b="0" textRotation="0"/>
+          <pm:cellMargin xmlns:pm="smNativeData" id="1579466201" l="0" r="384" t="0" b="0" textRotation="0"/>
         </ext>
       </extLst>
     </xf>
@@ -761,7 +791,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1573936295" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1579466201" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -1253,7 +1283,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1262,14 +1292,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1508,7 +1538,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1517,14 +1547,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1795,7 +1825,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1804,14 +1834,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2083,7 +2113,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2092,14 +2122,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2110,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:L13"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -2563,46 +2593,265 @@
       <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="11" t="n">
+      <c r="C13" s="24" t="n">
         <v>37.2999999999999972</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="24" t="n">
         <v>40.7000000000000028</v>
       </c>
-      <c r="E13" s="11" t="n">
+      <c r="E13" s="24" t="n">
         <v>31.8999999999999986</v>
       </c>
-      <c r="F13" s="11" t="n">
+      <c r="F13" s="24" t="n">
         <v>34.2000000000000028</v>
       </c>
-      <c r="G13" s="11" t="n">
+      <c r="G13" s="24" t="n">
         <v>41.7999999999999972</v>
       </c>
-      <c r="H13" s="11" t="n">
+      <c r="H13" s="24" t="n">
         <v>38.5</v>
       </c>
-      <c r="I13" s="11" t="n">
+      <c r="I13" s="24" t="n">
         <v>40.8999999999999986</v>
       </c>
-      <c r="J13" s="11" t="n">
+      <c r="J13" s="24" t="n">
         <v>37.6000000000000014</v>
       </c>
-      <c r="K13" s="11" t="n">
+      <c r="K13" s="24" t="n">
         <v>35.3999999999999986</v>
       </c>
-      <c r="L13" s="11" t="n">
+      <c r="L13" s="24" t="n">
         <v>38.1000000000000014</v>
       </c>
     </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="34" t="n">
+        <v>4.17999999999999972</v>
+      </c>
+      <c r="D14" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="34" t="n">
+        <v>4.16000000000000014</v>
+      </c>
+      <c r="F14" s="34" t="n">
+        <v>2.04000000000000004</v>
+      </c>
+      <c r="G14" s="34" t="n">
+        <v>3.00999999999999979</v>
+      </c>
+      <c r="H14" s="34" t="n">
+        <v>3.58999999999999986</v>
+      </c>
+      <c r="I14" s="34" t="n">
+        <v>4.94000000000000039</v>
+      </c>
+      <c r="J14" s="34" t="n">
+        <v>4.51159999999999961</v>
+      </c>
+      <c r="K14" s="34" t="n">
+        <v>2.13949999999999996</v>
+      </c>
+      <c r="L14" s="34" t="n">
+        <v>3.3266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="13"/>
+      <c r="B15" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="34" t="n">
+        <v>6.38999999999999968</v>
+      </c>
+      <c r="D15" s="34" t="n">
+        <v>7.48000000000000043</v>
+      </c>
+      <c r="E15" s="34" t="n">
+        <v>7.37999999999999989</v>
+      </c>
+      <c r="F15" s="34" t="n">
+        <v>6.91999999999999993</v>
+      </c>
+      <c r="G15" s="34" t="n">
+        <v>5.59999999999999964</v>
+      </c>
+      <c r="H15" s="34" t="n">
+        <v>7.00999999999999979</v>
+      </c>
+      <c r="I15" s="34" t="n">
+        <v>6.67999999999999972</v>
+      </c>
+      <c r="J15" s="34" t="n">
+        <v>7.63060000000000027</v>
+      </c>
+      <c r="K15" s="34" t="n">
+        <v>5.75570000000000004</v>
+      </c>
+      <c r="L15" s="34" t="n">
+        <v>5.16230000000000011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="13"/>
+      <c r="B16" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="34" t="n">
+        <v>11.2599999999999998</v>
+      </c>
+      <c r="D16" s="34" t="n">
+        <v>11.3100000000000005</v>
+      </c>
+      <c r="E16" s="34" t="n">
+        <v>9.44999999999999929</v>
+      </c>
+      <c r="F16" s="34" t="n">
+        <v>11.6899999999999995</v>
+      </c>
+      <c r="G16" s="34" t="n">
+        <v>7.95999999999999996</v>
+      </c>
+      <c r="H16" s="34" t="n">
+        <v>9.72000000000000064</v>
+      </c>
+      <c r="I16" s="34" t="n">
+        <v>9.82000000000000028</v>
+      </c>
+      <c r="J16" s="34" t="n">
+        <v>11.3369</v>
+      </c>
+      <c r="K16" s="34" t="n">
+        <v>10.0609000000000002</v>
+      </c>
+      <c r="L16" s="34" t="n">
+        <v>9.74810000000000088</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="13"/>
+      <c r="B17" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="34" t="n">
+        <v>15.2899999999999991</v>
+      </c>
+      <c r="D17" s="34" t="n">
+        <v>13.3900000000000006</v>
+      </c>
+      <c r="E17" s="34" t="n">
+        <v>12.5600000000000005</v>
+      </c>
+      <c r="F17" s="34" t="n">
+        <v>17.5300000000000011</v>
+      </c>
+      <c r="G17" s="34" t="n">
+        <v>14.7599999999999998</v>
+      </c>
+      <c r="H17" s="34" t="n">
+        <v>14.1799999999999997</v>
+      </c>
+      <c r="I17" s="34" t="n">
+        <v>15.3699999999999992</v>
+      </c>
+      <c r="J17" s="34" t="n">
+        <v>16.1246000000000009</v>
+      </c>
+      <c r="K17" s="34" t="n">
+        <v>16.1170000000000009</v>
+      </c>
+      <c r="L17" s="34" t="n">
+        <v>16.343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="13"/>
+      <c r="B18" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="34" t="n">
+        <v>20.4499999999999993</v>
+      </c>
+      <c r="D18" s="34" t="n">
+        <v>20.8200000000000003</v>
+      </c>
+      <c r="E18" s="34" t="n">
+        <v>16.4200000000000017</v>
+      </c>
+      <c r="F18" s="34" t="n">
+        <v>17.9299999999999997</v>
+      </c>
+      <c r="G18" s="34" t="n">
+        <v>18.6700000000000017</v>
+      </c>
+      <c r="H18" s="34" t="n">
+        <v>19.7100000000000009</v>
+      </c>
+      <c r="I18" s="34" t="n">
+        <v>20.6700000000000017</v>
+      </c>
+      <c r="J18" s="34" t="n">
+        <v>22.8871000000000002</v>
+      </c>
+      <c r="K18" s="34" t="n">
+        <v>25.2162000000000006</v>
+      </c>
+      <c r="L18" s="34" t="n">
+        <v>25.3381000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="13"/>
+      <c r="B19" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="34" t="n">
+        <v>37.2700000000000031</v>
+      </c>
+      <c r="D19" s="34" t="n">
+        <v>35.7299999999999969</v>
+      </c>
+      <c r="E19" s="34" t="n">
+        <v>34.9099999999999966</v>
+      </c>
+      <c r="F19" s="34" t="n">
+        <v>35.4799999999999969</v>
+      </c>
+      <c r="G19" s="34" t="n">
+        <v>32.8699999999999974</v>
+      </c>
+      <c r="H19" s="34" t="n">
+        <v>37.2999999999999972</v>
+      </c>
+      <c r="I19" s="34" t="n">
+        <v>42.1400000000000006</v>
+      </c>
+      <c r="J19" s="34" t="n">
+        <v>41.7492999999999981</v>
+      </c>
+      <c r="K19" s="34" t="n">
+        <v>39.6540999999999997</v>
+      </c>
+      <c r="L19" s="34" t="n">
+        <v>43.7541000000000011</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2611,14 +2860,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2631,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2643,7 +2892,7 @@
   <sheetData>
     <row r="1" spans="2:12">
       <c r="B1" s="16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="17" t="n">
         <v>1989</v>
@@ -3042,7 +3291,7 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>1</v>
@@ -3086,31 +3335,31 @@
       <c r="C13" s="29" t="n">
         <v>5.29999999999999982</v>
       </c>
-      <c r="D13" s="30" t="n">
+      <c r="D13" s="2" t="n">
         <v>5.5</v>
       </c>
-      <c r="E13" s="30" t="n">
+      <c r="E13" s="2" t="n">
         <v>5.40000000000000036</v>
       </c>
-      <c r="F13" s="30" t="n">
+      <c r="F13" s="2" t="n">
         <v>5.90000000000000036</v>
       </c>
-      <c r="G13" s="30" t="n">
+      <c r="G13" s="2" t="n">
         <v>4.5</v>
       </c>
-      <c r="H13" s="30" t="n">
+      <c r="H13" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="I13" s="30" t="n">
+      <c r="I13" s="2" t="n">
         <v>7.09999999999999964</v>
       </c>
-      <c r="J13" s="30" t="n">
+      <c r="J13" s="2" t="n">
         <v>4.59999999999999964</v>
       </c>
-      <c r="K13" s="30" t="n">
+      <c r="K13" s="2" t="n">
         <v>4.20000000000000018</v>
       </c>
-      <c r="L13" s="31" t="n">
+      <c r="L13" s="30" t="n">
         <v>4.40000000000000036</v>
       </c>
     </row>
@@ -3122,31 +3371,31 @@
       <c r="C14" s="29" t="n">
         <v>12.5</v>
       </c>
-      <c r="D14" s="30" t="n">
+      <c r="D14" s="2" t="n">
         <v>11.6999999999999993</v>
       </c>
-      <c r="E14" s="30" t="n">
+      <c r="E14" s="2" t="n">
         <v>11.0999999999999996</v>
       </c>
-      <c r="F14" s="30" t="n">
+      <c r="F14" s="2" t="n">
         <v>11.8000000000000007</v>
       </c>
-      <c r="G14" s="30" t="n">
+      <c r="G14" s="2" t="n">
         <v>12.8000000000000007</v>
       </c>
-      <c r="H14" s="30" t="n">
+      <c r="H14" s="2" t="n">
         <v>12.5999999999999996</v>
       </c>
-      <c r="I14" s="30" t="n">
+      <c r="I14" s="2" t="n">
         <v>11.9000000000000004</v>
       </c>
-      <c r="J14" s="30" t="n">
+      <c r="J14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="K14" s="30" t="n">
+      <c r="K14" s="2" t="n">
         <v>12.9000000000000004</v>
       </c>
-      <c r="L14" s="31" t="n">
+      <c r="L14" s="30" t="n">
         <v>13.5999999999999996</v>
       </c>
     </row>
@@ -3158,31 +3407,31 @@
       <c r="C15" s="29" t="n">
         <v>26</v>
       </c>
-      <c r="D15" s="30" t="n">
+      <c r="D15" s="2" t="n">
         <v>23.3999999999999986</v>
       </c>
-      <c r="E15" s="30" t="n">
+      <c r="E15" s="2" t="n">
         <v>21.1999999999999993</v>
       </c>
-      <c r="F15" s="30" t="n">
+      <c r="F15" s="2" t="n">
         <v>26.1999999999999993</v>
       </c>
-      <c r="G15" s="30" t="n">
+      <c r="G15" s="2" t="n">
         <v>19.5</v>
       </c>
-      <c r="H15" s="30" t="n">
+      <c r="H15" s="2" t="n">
         <v>23.1000000000000014</v>
       </c>
-      <c r="I15" s="30" t="n">
+      <c r="I15" s="2" t="n">
         <v>26.3999999999999986</v>
       </c>
-      <c r="J15" s="30" t="n">
+      <c r="J15" s="2" t="n">
         <v>27.1000000000000014</v>
       </c>
-      <c r="K15" s="30" t="n">
+      <c r="K15" s="2" t="n">
         <v>25.6000000000000014</v>
       </c>
-      <c r="L15" s="31" t="n">
+      <c r="L15" s="30" t="n">
         <v>26.1999999999999993</v>
       </c>
     </row>
@@ -3191,7 +3440,7 @@
       <c r="B16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="32" t="n">
+      <c r="C16" s="31" t="n">
         <v>44.7000000000000028</v>
       </c>
       <c r="D16" s="7" t="n">
@@ -3218,7 +3467,7 @@
       <c r="K16" s="7" t="n">
         <v>44.8999999999999986</v>
       </c>
-      <c r="L16" s="33" t="n">
+      <c r="L16" s="32" t="n">
         <v>51.2999999999999972</v>
       </c>
     </row>
@@ -3231,7 +3480,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3240,14 +3489,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -3273,7 +3522,7 @@
   <sheetData>
     <row r="1" spans="2:12">
       <c r="B1" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C1" s="9" t="n">
         <v>1989</v>
@@ -3526,7 +3775,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>7</v>
@@ -3750,7 +3999,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573936295" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1579466201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3759,14 +4008,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573936295" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1579466201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573936295" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1579466201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>